<commit_message>
:nut_and_bolt: fix failing atomic tabOTTR tests due to breaking change.
</commit_message>
<xml_diff>
--- a/lutra-tab/src/test/resources/atomic/typedBooleans.xlsx
+++ b/lutra-tab/src/test/resources/atomic/typedBooleans.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,10 +43,10 @@
     <t xml:space="preserve">ex:NoTemplate</t>
   </si>
   <si>
+    <t xml:space="preserve">xsd:boolean</t>
+  </si>
+  <si>
     <t xml:space="preserve">data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xsd:boolean</t>
   </si>
 </sst>
 </file>
@@ -177,12 +177,12 @@
   <dimension ref="A2:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -225,13 +225,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>1</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -258,7 +258,7 @@
       <c r="C11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>